<commit_message>
Burn down sowie Doku für Iteration III
</commit_message>
<xml_diff>
--- a/swe-iot/docs/BurnDown_Charts.xlsx
+++ b/swe-iot/docs/BurnDown_Charts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>BurndownChart</t>
   </si>
@@ -1017,6 +1017,493 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-AT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Burn Down</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> IT III</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal Tasks Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$38:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.510416666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.520833333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.541666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$38:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Tasks Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$38:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.510416666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.520833333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.541666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$38:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$D$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$38:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.510416666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.520833333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.541666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$D$38:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2005909808"/>
+        <c:axId val="-2033472960"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2005909808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2033472960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2033472960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2005909808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1097,6 +1584,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1614,6 +2141,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2186,6 +3229,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2457,10 +3530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2609,6 +3682,74 @@
         <v>0</v>
       </c>
     </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B38" s="3">
+        <v>4</v>
+      </c>
+      <c r="C38" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="B39" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="C39" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>0.52083333333333304</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="C40" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>0.53125</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Iteration IV Doku und Burn D. Chart
</commit_message>
<xml_diff>
--- a/swe-iot/docs/BurnDown_Charts.xlsx
+++ b/swe-iot/docs/BurnDown_Charts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>BurndownChart</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>Iteration I</t>
+  </si>
+  <si>
+    <t>Iteration IV</t>
+  </si>
+  <si>
+    <t>Iteration III</t>
   </si>
 </sst>
 </file>
@@ -1504,6 +1510,405 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-AT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal Tasks Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$56:$A$60</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.552083333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.572916666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.583333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$56:$B$60</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Tasks Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$56:$A$60</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.552083333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.572916666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.583333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$56:$C$60</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2006909792"/>
+        <c:axId val="-2006518656"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2006909792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2006518656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2006518656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2006909792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1624,6 +2029,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2657,6 +3102,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3259,6 +4220,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Diagramm 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3530,15 +4521,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -3684,7 +4676,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -3748,6 +4740,74 @@
       </c>
       <c r="C42" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="B56" s="3">
+        <v>3</v>
+      </c>
+      <c r="C56" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="B57" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="C57" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>0.57291666666666696</v>
+      </c>
+      <c r="B58" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C58" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="B59" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C59" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>0.59375</v>
+      </c>
+      <c r="B60" s="3">
+        <v>0</v>
+      </c>
+      <c r="C60" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Doku und Burndown für Iteration V
</commit_message>
<xml_diff>
--- a/swe-iot/docs/BurnDown_Charts.xlsx
+++ b/swe-iot/docs/BurnDown_Charts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>BurndownChart</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Iteration III</t>
+  </si>
+  <si>
+    <t>Iteration V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kein Burn Down Chart -  keine Epics umgesetzt </t>
   </si>
 </sst>
 </file>
@@ -4521,10 +4527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4810,6 +4816,41 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="2"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="2"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="2"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="2"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="2"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>